<commit_message>
Editted bug ft Jerk
</commit_message>
<xml_diff>
--- a/Files/Tabellenboek.xlsx
+++ b/Files/Tabellenboek.xlsx
@@ -89,10 +89,10 @@
     <t>1. Dit is een normale SR Vraag</t>
   </si>
   <si>
-    <t>V1</t>
-  </si>
-  <si>
-    <t>V2</t>
+    <t>KV1</t>
+  </si>
+  <si>
+    <t>KV2</t>
   </si>
   <si>
     <t>Properties (%)</t>

</xml_diff>

<commit_message>
Newest Version, remove print statements
</commit_message>
<xml_diff>
--- a/Files/Tabellenboek.xlsx
+++ b/Files/Tabellenboek.xlsx
@@ -89,10 +89,10 @@
     <t>1. Dit is een normale SR Vraag</t>
   </si>
   <si>
-    <t>KV1</t>
-  </si>
-  <si>
-    <t>KV2</t>
+    <t>V1</t>
+  </si>
+  <si>
+    <t>V2</t>
   </si>
   <si>
     <t>Properties (%)</t>
@@ -470,31 +470,31 @@
     <t>Test3</t>
   </si>
   <si>
-    <t>V1:    1. Dit is een normale SR Vraag</t>
-  </si>
-  <si>
-    <t>V2:    2. Dit is een SR Vraag + Anders, namelijk</t>
-  </si>
-  <si>
-    <t>OPEN2_5:    2. Dit is een SR Vraag + Anders, namelijk A:5</t>
-  </si>
-  <si>
-    <t>OPEN7_5:    Anders, namelijk:</t>
-  </si>
-  <si>
-    <t>OPEN8_5:    Anders, namelijk:</t>
-  </si>
-  <si>
-    <t>V18_A1:    18-1. Antwoord 1</t>
-  </si>
-  <si>
-    <t>V18_A2:    18-2. Antwoord 2</t>
-  </si>
-  <si>
-    <t>V18_A3:    18-3. Antwoord 3</t>
-  </si>
-  <si>
-    <t>V19:    19. Dit is een open vraag</t>
+    <t>V1:    . Dit is een normale SR Vraag</t>
+  </si>
+  <si>
+    <t>V2:    . Dit is een SR Vraag + Anders, namelijk</t>
+  </si>
+  <si>
+    <t>OPEN2_5:    . Dit is een SR Vraag + Anders, namelijk A:5</t>
+  </si>
+  <si>
+    <t>OPEN7_5:    nders, namelijk:</t>
+  </si>
+  <si>
+    <t>OPEN8_5:    nders, namelijk:</t>
+  </si>
+  <si>
+    <t>V18_A1:    8-1. Antwoord 1</t>
+  </si>
+  <si>
+    <t>V18_A2:    8-2. Antwoord 2</t>
+  </si>
+  <si>
+    <t>V18_A3:    8-3. Antwoord 3</t>
+  </si>
+  <si>
+    <t>V19:    9. Dit is een open vraag</t>
   </si>
 </sst>
 </file>
@@ -777,15 +777,15 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:I8" totalsRowShown="0">
   <autoFilter ref="A1:I8"/>
   <tableColumns count="9">
-    <tableColumn id="1" name="V1:    1. Dit is een normale SR Vraag"/>
-    <tableColumn id="2" name="V2:    2. Dit is een SR Vraag + Anders, namelijk"/>
-    <tableColumn id="3" name="OPEN2_5:    2. Dit is een SR Vraag + Anders, namelijk A:5"/>
-    <tableColumn id="4" name="OPEN7_5:    Anders, namelijk:"/>
-    <tableColumn id="5" name="OPEN8_5:    Anders, namelijk:"/>
-    <tableColumn id="6" name="V18_A1:    18-1. Antwoord 1"/>
-    <tableColumn id="7" name="V18_A2:    18-2. Antwoord 2"/>
-    <tableColumn id="8" name="V18_A3:    18-3. Antwoord 3"/>
-    <tableColumn id="9" name="V19:    19. Dit is een open vraag"/>
+    <tableColumn id="1" name="V1:    . Dit is een normale SR Vraag"/>
+    <tableColumn id="2" name="V2:    . Dit is een SR Vraag + Anders, namelijk"/>
+    <tableColumn id="3" name="OPEN2_5:    . Dit is een SR Vraag + Anders, namelijk A:5"/>
+    <tableColumn id="4" name="OPEN7_5:    nders, namelijk:"/>
+    <tableColumn id="5" name="OPEN8_5:    nders, namelijk:"/>
+    <tableColumn id="6" name="V18_A1:    8-1. Antwoord 1"/>
+    <tableColumn id="7" name="V18_A2:    8-2. Antwoord 2"/>
+    <tableColumn id="8" name="V18_A3:    8-3. Antwoord 3"/>
+    <tableColumn id="9" name="V19:    9. Dit is een open vraag"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>

</xml_diff>